<commit_message>
Pierwsza stabilna wersja bez instrukcji
</commit_message>
<xml_diff>
--- a/Przelicznik.xlsx
+++ b/Przelicznik.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kwiec\Desktop\AREX\Programy\Przelicznik wagowy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB3DFAE-DECB-4A74-B3D1-8C0E051694FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A15E52-D4CF-4833-99DD-75861B1A4AD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6022" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6014" uniqueCount="60">
   <si>
     <t>1000 SZT/KG</t>
   </si>
@@ -29723,15 +29723,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39D17DA-1483-46D4-888D-55DBC95BDBF7}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="54" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="36" x14ac:dyDescent="0.35">
       <c r="A1" s="101" t="s">
         <v>0</v>
       </c>
@@ -30371,7 +30371,7 @@
     </row>
     <row r="23" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A23" s="100">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B23" s="98" t="s">
         <v>57</v>
@@ -30400,7 +30400,7 @@
     </row>
     <row r="24" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A24" s="100">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B24" s="98" t="s">
         <v>57</v>
@@ -30429,7 +30429,7 @@
     </row>
     <row r="25" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A25" s="100">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B25" s="98" t="s">
         <v>57</v>
@@ -30458,7 +30458,7 @@
     </row>
     <row r="26" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="100">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="B26" s="98" t="s">
         <v>57</v>
@@ -30482,35 +30482,6 @@
         <v>57</v>
       </c>
       <c r="I26" s="98" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A27" s="100">
-        <v>100</v>
-      </c>
-      <c r="B27" s="98" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" s="103" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="99" t="s">
-        <v>57</v>
-      </c>
-      <c r="E27" s="98" t="s">
-        <v>57</v>
-      </c>
-      <c r="F27" s="99" t="s">
-        <v>57</v>
-      </c>
-      <c r="G27" s="98" t="s">
-        <v>57</v>
-      </c>
-      <c r="H27" s="99" t="s">
-        <v>57</v>
-      </c>
-      <c r="I27" s="98" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Wersja z instrukcją 2/3
</commit_message>
<xml_diff>
--- a/Przelicznik.xlsx
+++ b/Przelicznik.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kwiec\Desktop\AREX\Programy\Przelicznik wagowy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A15E52-D4CF-4833-99DD-75861B1A4AD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97EB4BBC-DCE9-4CA4-AFDD-561CA3F26829}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DIN 933" sheetId="1" r:id="rId1"/>
@@ -17157,13 +17157,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C68C2476-D9C4-4078-BA70-396F8236A40D}">
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:P47"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16" ht="54" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="36" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -29725,7 +29725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39D17DA-1483-46D4-888D-55DBC95BDBF7}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>

</xml_diff>